<commit_message>
Updated version of the data
</commit_message>
<xml_diff>
--- a/grouped table of annotations.xlsx
+++ b/grouped table of annotations.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0.sharepoint.com/sites/PEJUS685/Documentos compartidos/General/BPI Challenge/Artículo/Material suplementario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{14FC0707-65B5-4CA3-BA7A-BDA05980EF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3205D1A5-AC8B-4D30-B228-94AFE28AB89E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E11A9B1-6FBE-45B3-A889-8B25E8F8C9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk84405051" localSheetId="0">Sheet1!$CN$5</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="268">
   <si>
     <t>A1 P2 BPI 2020</t>
   </si>
@@ -480,9 +483,6 @@
     <t>Identify impact of bottlenecks by organizational unit</t>
   </si>
   <si>
-    <t>Grouping traces by cycle time</t>
-  </si>
-  <si>
     <t>Filter events by attributes</t>
   </si>
   <si>
@@ -558,9 +558,6 @@
     <t>Calculate Statistics of attributes</t>
   </si>
   <si>
-    <t>Grouping by organizational units</t>
-  </si>
-  <si>
     <t>Calculate dates of the development of activities of resources</t>
   </si>
   <si>
@@ -610,13 +607,244 @@
   </si>
   <si>
     <t>Apply decision trees</t>
+  </si>
+  <si>
+    <t>A6 P5 BPI 2015</t>
+  </si>
+  <si>
+    <t>Identify organizational units by cycle time</t>
+  </si>
+  <si>
+    <t>Group traces by sub-processes</t>
+  </si>
+  <si>
+    <t>A12 P1 BPI 2017</t>
+  </si>
+  <si>
+    <t>Identify transitions by cycle time</t>
+  </si>
+  <si>
+    <t>Group traces by endpoints</t>
+  </si>
+  <si>
+    <t>Group traces by cycle time</t>
+  </si>
+  <si>
+    <t>Identify common activities</t>
+  </si>
+  <si>
+    <t>Calculate frequency of sub-processes</t>
+  </si>
+  <si>
+    <t>Represent linear tendency of cycle time</t>
+  </si>
+  <si>
+    <t>A19 P1 BPI 2017</t>
+  </si>
+  <si>
+    <t>Filter activities by resource</t>
+  </si>
+  <si>
+    <t>A2 P2 BPI 2019</t>
+  </si>
+  <si>
+    <t>Identify attributes by cycle time</t>
+  </si>
+  <si>
+    <t>A11 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>Represent temporal series of traces</t>
+  </si>
+  <si>
+    <t>Filter traces by year</t>
+  </si>
+  <si>
+    <t>Calculate number of sub-processes</t>
+  </si>
+  <si>
+    <t>Filter sub-processes by cycle time</t>
+  </si>
+  <si>
+    <t>Calculate percentage of sub-processes</t>
+  </si>
+  <si>
+    <t>Represent bar charts of sub-processes</t>
+  </si>
+  <si>
+    <t>Filter sub-processes by attributes</t>
+  </si>
+  <si>
+    <t>Group sub-processes</t>
+  </si>
+  <si>
+    <t>A16 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>A16 P3 BPI 2020</t>
+  </si>
+  <si>
+    <t>Calculate frequency of traces</t>
+  </si>
+  <si>
+    <t>A16 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>A16 P5 BPI 2020</t>
+  </si>
+  <si>
+    <t>A16 P6 BPI 2020</t>
+  </si>
+  <si>
+    <t>Identify traces by cycle time</t>
+  </si>
+  <si>
+    <t>A24 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>A24 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>Compare processing time</t>
+  </si>
+  <si>
+    <t>A24 P4 BPI 2020</t>
+  </si>
+  <si>
+    <t>A1 P5 BPI 2015</t>
+  </si>
+  <si>
+    <t>Identify organizational units by traces</t>
+  </si>
+  <si>
+    <t>Group traces by resources</t>
+  </si>
+  <si>
+    <t>Calculate percentage of activities</t>
+  </si>
+  <si>
+    <t>A5 P5 BPI 2015</t>
+  </si>
+  <si>
+    <t>Identify organizational units by resources</t>
+  </si>
+  <si>
+    <t>A3 P1 BPI 2017</t>
+  </si>
+  <si>
+    <t>A18 P1 BPI 2017</t>
+  </si>
+  <si>
+    <t>Filter events by resources</t>
+  </si>
+  <si>
+    <t>Identify attributes by traces</t>
+  </si>
+  <si>
+    <t>Group events by attributes</t>
+  </si>
+  <si>
+    <t>A9 P2 BPI 2019</t>
+  </si>
+  <si>
+    <t>A12 P2 BPI 2019</t>
+  </si>
+  <si>
+    <t>A30 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>A31 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>A34 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>Filter traces by subprocesses</t>
+  </si>
+  <si>
+    <t>A27 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>Represent bart charts of activities</t>
+  </si>
+  <si>
+    <t>A30 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>Group traces by month</t>
+  </si>
+  <si>
+    <t>A31 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>A19 P4 BPI 2020</t>
+  </si>
+  <si>
+    <t>Represent temporal series of activities</t>
+  </si>
+  <si>
+    <t>Identify activities with cycle time</t>
+  </si>
+  <si>
+    <t>Identify roles by organizational units</t>
+  </si>
+  <si>
+    <t>Identify activities with traces</t>
+  </si>
+  <si>
+    <t>A27 P4 BPI 2020</t>
+  </si>
+  <si>
+    <t>A31 P4 BPI 2020</t>
+  </si>
+  <si>
+    <t>A19 P5 BPI 2020</t>
+  </si>
+  <si>
+    <t>A30 P5 BPI 2020</t>
+  </si>
+  <si>
+    <t>A34 P5 BPI 2020</t>
+  </si>
+  <si>
+    <t>Identify activities as bottlenecks applying temporal performance criteria and statistical measures</t>
+  </si>
+  <si>
+    <t>A30 P6 BPI 2020</t>
+  </si>
+  <si>
+    <t>Represent lineal distribution of an attribute by traces</t>
+  </si>
+  <si>
+    <t>A19 P1 BPI 2020</t>
+  </si>
+  <si>
+    <t>Calculate Statistics of activities</t>
+  </si>
+  <si>
+    <t>Represent temporal series of throughput</t>
+  </si>
+  <si>
+    <t>Represent correlation graph of variables</t>
+  </si>
+  <si>
+    <t>Group traces by organizational units</t>
+  </si>
+  <si>
+    <t>A11 P5 BPI 2020</t>
+  </si>
+  <si>
+    <t>A11 P2 BPI 2020</t>
+  </si>
+  <si>
+    <t>A11 P4 BPI 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +867,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -648,7 +895,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -671,11 +918,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -694,6 +952,44 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,57 +1329,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CM24"/>
+  <dimension ref="A1:DW58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE9" workbookViewId="0">
-      <selection activeCell="CI11" sqref="CI11"/>
+    <sheetView tabSelected="1" topLeftCell="CN8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CP13" sqref="CP13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.453125" customWidth="1"/>
-    <col min="3" max="3" width="56.26953125" customWidth="1"/>
-    <col min="4" max="4" width="47.453125" customWidth="1"/>
-    <col min="5" max="5" width="47.54296875" customWidth="1"/>
-    <col min="6" max="6" width="51.26953125" customWidth="1"/>
-    <col min="7" max="7" width="46.54296875" customWidth="1"/>
-    <col min="8" max="8" width="42.1796875" customWidth="1"/>
-    <col min="9" max="9" width="72.26953125" customWidth="1"/>
-    <col min="10" max="10" width="46.26953125" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="8" max="8" width="42.140625" customWidth="1"/>
+    <col min="9" max="9" width="72.28515625" customWidth="1"/>
+    <col min="10" max="10" width="46.28515625" customWidth="1"/>
     <col min="11" max="11" width="39" customWidth="1"/>
-    <col min="12" max="12" width="44.26953125" customWidth="1"/>
-    <col min="13" max="13" width="49.453125" customWidth="1"/>
-    <col min="14" max="14" width="58.453125" customWidth="1"/>
-    <col min="15" max="15" width="28.453125" customWidth="1"/>
+    <col min="12" max="12" width="44.28515625" customWidth="1"/>
+    <col min="13" max="13" width="49.42578125" customWidth="1"/>
+    <col min="14" max="14" width="58.42578125" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" customWidth="1"/>
     <col min="16" max="16" width="32" customWidth="1"/>
-    <col min="17" max="17" width="73.54296875" customWidth="1"/>
-    <col min="18" max="18" width="58.81640625" customWidth="1"/>
-    <col min="19" max="19" width="46.26953125" customWidth="1"/>
-    <col min="20" max="20" width="32.81640625" customWidth="1"/>
+    <col min="17" max="17" width="73.5703125" customWidth="1"/>
+    <col min="18" max="18" width="58.85546875" customWidth="1"/>
+    <col min="19" max="19" width="46.28515625" customWidth="1"/>
+    <col min="20" max="20" width="32.85546875" customWidth="1"/>
     <col min="21" max="21" width="74" customWidth="1"/>
-    <col min="22" max="22" width="75.453125" customWidth="1"/>
-    <col min="23" max="23" width="56.54296875" customWidth="1"/>
-    <col min="24" max="24" width="103.26953125" customWidth="1"/>
-    <col min="25" max="25" width="68.54296875" customWidth="1"/>
-    <col min="26" max="26" width="57.26953125" customWidth="1"/>
-    <col min="27" max="27" width="55.54296875" customWidth="1"/>
-    <col min="28" max="28" width="51.26953125" customWidth="1"/>
-    <col min="29" max="29" width="40.453125" customWidth="1"/>
-    <col min="30" max="30" width="55.453125" customWidth="1"/>
-    <col min="31" max="31" width="54.1796875" customWidth="1"/>
-    <col min="32" max="32" width="38.1796875" customWidth="1"/>
-    <col min="33" max="33" width="25.453125" customWidth="1"/>
-    <col min="34" max="34" width="56.81640625" customWidth="1"/>
-    <col min="35" max="35" width="30.7265625" customWidth="1"/>
-    <col min="36" max="36" width="43.1796875" customWidth="1"/>
-    <col min="37" max="37" width="42.54296875" customWidth="1"/>
-    <col min="38" max="38" width="23.7265625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="75.42578125" customWidth="1"/>
+    <col min="23" max="23" width="56.5703125" customWidth="1"/>
+    <col min="24" max="24" width="103.28515625" customWidth="1"/>
+    <col min="25" max="25" width="68.5703125" customWidth="1"/>
+    <col min="26" max="26" width="57.28515625" customWidth="1"/>
+    <col min="27" max="27" width="55.5703125" customWidth="1"/>
+    <col min="28" max="28" width="51.28515625" customWidth="1"/>
+    <col min="29" max="29" width="40.42578125" customWidth="1"/>
+    <col min="30" max="30" width="55.42578125" customWidth="1"/>
+    <col min="31" max="31" width="54.140625" customWidth="1"/>
+    <col min="32" max="32" width="38.140625" customWidth="1"/>
+    <col min="33" max="33" width="25.42578125" customWidth="1"/>
+    <col min="34" max="34" width="56.85546875" customWidth="1"/>
+    <col min="35" max="35" width="30.7109375" customWidth="1"/>
+    <col min="36" max="36" width="43.140625" customWidth="1"/>
+    <col min="37" max="37" width="42.5703125" customWidth="1"/>
+    <col min="38" max="38" width="23.7109375" style="4" customWidth="1"/>
     <col min="39" max="82" width="19" style="4" customWidth="1"/>
     <col min="83" max="83" width="30" style="4" customWidth="1"/>
     <col min="84" max="91" width="19" style="4" customWidth="1"/>
+    <col min="92" max="92" width="31.85546875" customWidth="1"/>
+    <col min="93" max="93" width="24.5703125" customWidth="1"/>
+    <col min="94" max="94" width="24.42578125" customWidth="1"/>
+    <col min="95" max="95" width="26.140625" customWidth="1"/>
+    <col min="96" max="96" width="20.42578125" customWidth="1"/>
+    <col min="97" max="98" width="25.42578125" customWidth="1"/>
+    <col min="99" max="99" width="28.28515625" customWidth="1"/>
+    <col min="100" max="100" width="26.5703125" customWidth="1"/>
+    <col min="101" max="101" width="26.85546875" customWidth="1"/>
+    <col min="102" max="102" width="25.42578125" customWidth="1"/>
+    <col min="103" max="103" width="26" customWidth="1"/>
+    <col min="104" max="104" width="26.5703125" customWidth="1"/>
+    <col min="105" max="105" width="27.85546875" customWidth="1"/>
+    <col min="106" max="106" width="22.42578125" customWidth="1"/>
+    <col min="107" max="107" width="24.28515625" customWidth="1"/>
+    <col min="108" max="108" width="32.42578125" style="4" customWidth="1"/>
+    <col min="109" max="109" width="31.140625" style="4" customWidth="1"/>
+    <col min="110" max="110" width="27" customWidth="1"/>
+    <col min="111" max="111" width="21" customWidth="1"/>
+    <col min="112" max="112" width="32.7109375" customWidth="1"/>
+    <col min="113" max="113" width="33.42578125" customWidth="1"/>
+    <col min="114" max="114" width="35.7109375" customWidth="1"/>
+    <col min="115" max="115" width="25.7109375" customWidth="1"/>
+    <col min="116" max="116" width="27.85546875" customWidth="1"/>
+    <col min="117" max="117" width="24.7109375" customWidth="1"/>
+    <col min="118" max="118" width="27.42578125" customWidth="1"/>
+    <col min="119" max="119" width="26.85546875" customWidth="1"/>
+    <col min="120" max="120" width="25" customWidth="1"/>
+    <col min="121" max="121" width="25.7109375" customWidth="1"/>
+    <col min="122" max="122" width="32.140625" customWidth="1"/>
+    <col min="123" max="123" width="38.140625" customWidth="1"/>
+    <col min="124" max="124" width="33.85546875" customWidth="1"/>
+    <col min="125" max="125" width="30.5703125" customWidth="1"/>
+    <col min="126" max="126" width="26.42578125" customWidth="1"/>
+    <col min="127" max="127" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1354,8 +1685,116 @@
       <c r="CM1" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="CO1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="CP1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="CQ1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="CS1" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="CT1" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="CU1" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="CV1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="CW1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="CX1" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="CY1" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="CZ1" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="DA1" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="DB1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="DC1" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="DD1" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="DE1" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="DF1" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="DG1" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="DH1" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="DI1" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="DJ1" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="DK1" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="DL1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="DM1" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="DN1" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="DO1" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="DP1" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="DQ1" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="DR1" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="DS1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="DT1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="DU1" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="DV1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="DW1" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1629,8 +2068,116 @@
       <c r="CM2" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CO2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CP2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="CQ2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CS2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="CT2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="CU2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="CV2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="CW2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CY2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CZ2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="DA2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="DB2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="DC2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="DD2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="DE2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="DF2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="DG2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="DH2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="DI2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="DJ2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="DK2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="DL2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DM2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="DN2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="DO2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="DQ2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="DR2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DS2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="DT2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="DU2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="DV2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="DW2" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1889,8 +2436,113 @@
       <c r="CM3" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:91" ht="58" x14ac:dyDescent="0.35">
+      <c r="CN3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="CO3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="CP3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="CQ3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CR3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="CT3" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="CU3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="CW3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="CX3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="CY3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="CZ3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="DA3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="DB3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="DC3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD3" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="DE3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="DF3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="DG3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="DI3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="DJ3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="DK3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DL3" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="DM3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="DN3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DP3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="DQ3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="DR3" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="DS3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="DT3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="DU3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DV3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="DW3" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:127" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1991,7 +2643,7 @@
         <v>120</v>
       </c>
       <c r="BA4" s="4" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="BB4" s="4" t="s">
         <v>92</v>
@@ -2027,7 +2679,7 @@
         <v>122</v>
       </c>
       <c r="BN4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BO4" s="4" t="s">
         <v>104</v>
@@ -2042,10 +2694,10 @@
         <v>129</v>
       </c>
       <c r="BS4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="BT4" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="BT4" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="BU4" s="4" t="s">
         <v>137</v>
@@ -2060,7 +2712,7 @@
         <v>138</v>
       </c>
       <c r="BY4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BZ4" s="4" t="s">
         <v>116</v>
@@ -2072,7 +2724,7 @@
         <v>90</v>
       </c>
       <c r="CC4" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="CD4" s="4" t="s">
         <v>101</v>
@@ -2081,7 +2733,7 @@
         <v>127</v>
       </c>
       <c r="CF4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG4" s="4" t="s">
         <v>104</v>
@@ -2099,21 +2751,114 @@
         <v>139</v>
       </c>
       <c r="CL4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CM4" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CO4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="CP4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="CQ4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="CR4" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CT4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="CU4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="CV4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="CW4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="CX4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="DA4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="DB4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="DC4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="DD4" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="DE4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="DF4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="DG4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="DH4" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="DI4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="DJ4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="DK4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="DL4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="DN4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="DP4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="DQ4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="DS4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="DT4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DU4" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="DV4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="DW4" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L5" t="s">
         <v>156</v>
-      </c>
-      <c r="L5" t="s">
-        <v>157</v>
       </c>
       <c r="O5" t="s">
         <v>115</v>
@@ -2128,22 +2873,22 @@
         <v>122</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AN5" s="4" t="s">
         <v>104</v>
       </c>
       <c r="AP5" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU5" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="AV5" s="4" t="s">
         <v>129</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX5" s="4" t="s">
         <v>123</v>
@@ -2155,7 +2900,7 @@
         <v>109</v>
       </c>
       <c r="BA5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="BB5" s="4" t="s">
         <v>110</v>
@@ -2164,10 +2909,10 @@
         <v>92</v>
       </c>
       <c r="BE5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG5" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="BH5" s="4" t="s">
         <v>93</v>
@@ -2191,10 +2936,10 @@
         <v>117</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BR5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BS5" s="4" t="s">
         <v>117</v>
@@ -2227,7 +2972,7 @@
         <v>129</v>
       </c>
       <c r="CC5" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="CD5" s="4" t="s">
         <v>126</v>
@@ -2236,7 +2981,7 @@
         <v>123</v>
       </c>
       <c r="CF5" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="CG5" s="4" t="s">
         <v>106</v>
@@ -2248,19 +2993,97 @@
         <v>138</v>
       </c>
       <c r="CJ5" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CK5" s="4" t="s">
         <v>104</v>
       </c>
       <c r="CL5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="CM5" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="6" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN5" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="CQ5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="CR5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CT5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="CW5" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="CX5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="DA5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="DC5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="DD5" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="DE5" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="DF5" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="DG5" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="DH5" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI5" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="DJ5" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="DK5" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="DL5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="DN5" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="DP5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="DS5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="DT5" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="DW5" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2268,7 +3091,7 @@
         <v>138</v>
       </c>
       <c r="O6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V6" t="s">
         <v>103</v>
@@ -2283,7 +3106,7 @@
         <v>115</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AU6" s="4" t="s">
         <v>132</v>
@@ -2295,16 +3118,16 @@
         <v>129</v>
       </c>
       <c r="AZ6" s="4" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="BA6" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BB6" s="4" t="s">
         <v>128</v>
       </c>
       <c r="BD6" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BG6" s="4" t="s">
         <v>104</v>
@@ -2319,7 +3142,7 @@
         <v>147</v>
       </c>
       <c r="BN6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BP6" s="4" t="s">
         <v>99</v>
@@ -2328,10 +3151,10 @@
         <v>129</v>
       </c>
       <c r="BR6" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BS6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BT6" s="4" t="s">
         <v>98</v>
@@ -2373,13 +3196,13 @@
         <v>110</v>
       </c>
       <c r="CH6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="CI6" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="CI6" s="4" t="s">
-        <v>172</v>
-      </c>
       <c r="CJ6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="CK6" s="4" t="s">
         <v>144</v>
@@ -2388,21 +3211,93 @@
         <v>128</v>
       </c>
       <c r="CM6" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="CN6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="CO6" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="CP6" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="CQ6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="CR6" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="CT6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU6" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="CW6" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="CX6" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="CY6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="DA6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="DC6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DD6" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="DE6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="DF6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DG6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="DH6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="DI6" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DJ6" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="DN6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="DP6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="DS6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="DT6" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="DW6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V7" t="s">
         <v>143</v>
       </c>
       <c r="W7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AJ7" s="4" t="s">
         <v>115</v>
@@ -2423,13 +3318,13 @@
         <v>99</v>
       </c>
       <c r="AZ7" s="4" t="s">
-        <v>175</v>
+        <v>264</v>
       </c>
       <c r="BA7" s="4" t="s">
         <v>122</v>
       </c>
       <c r="BD7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BG7" s="4" t="s">
         <v>109</v>
@@ -2438,7 +3333,7 @@
         <v>107</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BN7" s="4" t="s">
         <v>113</v>
@@ -2447,10 +3342,10 @@
         <v>113</v>
       </c>
       <c r="BQ7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="BR7" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="BR7" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="BS7" s="4" t="s">
         <v>117</v>
@@ -2459,7 +3354,7 @@
         <v>117</v>
       </c>
       <c r="BU7" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BV7" s="4" t="s">
         <v>99</v>
@@ -2480,7 +3375,7 @@
         <v>122</v>
       </c>
       <c r="CF7" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="CG7" s="4" t="s">
         <v>116</v>
@@ -2489,7 +3384,7 @@
         <v>132</v>
       </c>
       <c r="CJ7" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="CK7" s="4" t="s">
         <v>144</v>
@@ -2498,10 +3393,82 @@
         <v>126</v>
       </c>
       <c r="CM7" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:91" ht="58" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+      <c r="CN7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="CO7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="CP7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="CQ7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="CR7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CT7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU7" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="CW7" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="CX7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY7" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="DA7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="DC7" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="DD7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="DE7" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="DF7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DG7" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="DH7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="DI7" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="DJ7" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="DN7" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DP7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="DS7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="DT7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="DW7" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:127" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2512,7 +3479,7 @@
         <v>128</v>
       </c>
       <c r="W8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AW8" s="4" t="s">
         <v>99</v>
@@ -2563,7 +3530,7 @@
         <v>122</v>
       </c>
       <c r="CA8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="CE8" s="4" t="s">
         <v>125</v>
@@ -2589,13 +3556,79 @@
       <c r="CM8" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="CO8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="CP8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="CQ8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CR8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="CT8" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CU8" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="CW8" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CX8" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="CY8" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="DA8" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="DC8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DD8" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="DE8" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="DF8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DH8" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DI8" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="DN8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DP8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DS8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DT8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="DW8" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="V9" t="s">
         <v>143</v>
@@ -2604,19 +3637,19 @@
         <v>107</v>
       </c>
       <c r="AZ9" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="BA9" s="4" t="s">
         <v>123</v>
       </c>
       <c r="BD9" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BG9" s="4" t="s">
         <v>138</v>
       </c>
       <c r="BN9" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BP9" s="4" t="s">
         <v>111</v>
@@ -2625,7 +3658,7 @@
         <v>94</v>
       </c>
       <c r="BR9" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="BT9" s="4" t="s">
         <v>140</v>
@@ -2643,7 +3676,7 @@
         <v>111</v>
       </c>
       <c r="CE9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="CG9" s="4" t="s">
         <v>110</v>
@@ -2660,8 +3693,71 @@
       <c r="CM9" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN9" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP9" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="CQ9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CT9" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="CU9" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="CW9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="CY9" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="DA9" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="DC9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="DE9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="DF9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DH9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="DI9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="DN9" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DP9" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DS9" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DT9" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="DW9" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2687,13 +3783,13 @@
         <v>117</v>
       </c>
       <c r="BR10" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="BT10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BV10" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BX10" s="4" t="s">
         <v>135</v>
@@ -2702,25 +3798,85 @@
         <v>117</v>
       </c>
       <c r="CE10" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="CG10" s="4" t="s">
         <v>126</v>
       </c>
       <c r="CH10" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="CJ10" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CL10" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="CM10" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CN10" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="CO10" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="CP10" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="CR10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="CU10" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="CW10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CY10" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="DA10" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DC10" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="DD10" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="DE10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DF10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH10" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DI10" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DN10" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="DP10" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="DS10" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="DT10" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DW10" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2749,16 +3905,16 @@
         <v>107</v>
       </c>
       <c r="CA11" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="CG11" s="4" t="s">
         <v>110</v>
       </c>
       <c r="CH11" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="CJ11" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CL11" s="4" t="s">
         <v>110</v>
@@ -2766,8 +3922,68 @@
       <c r="CM11" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+      <c r="CN11" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="CO11" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="CP11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="CQ11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="CR11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU11" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="CW11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="CY11" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="DA11" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="DC11" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="DD11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="DE11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="DF11" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DH11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="DI11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="DN11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="DP11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="DS11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DT11" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DW11" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:127" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2775,7 +3991,7 @@
         <v>104</v>
       </c>
       <c r="AZ12" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BN12" s="4" t="s">
         <v>138</v>
@@ -2790,10 +4006,10 @@
         <v>127</v>
       </c>
       <c r="CH12" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="CJ12" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="CL12" s="4" t="s">
         <v>122</v>
@@ -2801,8 +4017,63 @@
       <c r="CM12" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:91" ht="58" x14ac:dyDescent="0.35">
+      <c r="CN12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="CO12" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="CP12" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="CQ12" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="CR12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU12" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="CY12" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="DA12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="DC12" s="10"/>
+      <c r="DD12" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="DE12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="DF12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="DI12" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="DN12" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="DP12" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DS12" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DT12" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DW12" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:127" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2816,27 +4087,72 @@
         <v>132</v>
       </c>
       <c r="BQ13" s="4" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="CH13" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="CJ13" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="CL13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="CM13" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:91" ht="58" x14ac:dyDescent="0.35">
+      <c r="CN13" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO13" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="CP13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="CQ13" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="CR13" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="CU13" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="CY13" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="DA13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="DD13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="DE13" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="DF13" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DH13" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DI13" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="DP13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DS13" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:127" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="AZ14" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BQ14" s="4" t="s">
         <v>122</v>
@@ -2848,13 +4164,55 @@
         <v>101</v>
       </c>
       <c r="CL14" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="CM14" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:91" ht="58" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="CO14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CP14" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="CQ14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR14" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="CU14" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="CY14" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="DA14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="DD14" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="DE14" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="DF14" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH14" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DI14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DP14" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DS14" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:127" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2871,13 +4229,46 @@
         <v>99</v>
       </c>
       <c r="CL15" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="CM15" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="1:91" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="CO15" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CQ15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="CR15" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="CU15" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="CY15" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="DA15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="DE15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="DF15" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DI15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DP15" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="DS15" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:127" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2888,47 +4279,106 @@
         <v>104</v>
       </c>
       <c r="CH16" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="CJ16" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="CL16" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="CM16" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="17" spans="1:91" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="CO16" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="CQ16" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CR16" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="CU16" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="CY16" s="9"/>
+      <c r="DA16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="DE16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DF16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="DI16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="DP16" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="DS16" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="AZ17" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="CH17" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="CJ17" s="4" t="s">
         <v>116</v>
       </c>
       <c r="CL17" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="CM17" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+      <c r="CO17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CQ17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR17" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="CU17" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="CY17" s="9"/>
+      <c r="DA17" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="DF17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DI17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="DP17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="DS17" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:123" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="CH18" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="CJ18" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="CL18" s="4" t="s">
         <v>110</v>
@@ -2936,82 +4386,454 @@
       <c r="CM18" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:91" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="CO18" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CQ18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR18" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU18" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="DA18" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DF18" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="DI18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="DP18" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="DS18" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="CH19" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="CL19" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+      <c r="CO19" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="CQ19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="CR19" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="CU19" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="DA19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="DF19" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="DI19" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="DP19" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="DS19" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:123" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="CH20" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="CL20" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="21" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+      <c r="CO20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CQ20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="CR20" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="CU20" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DA20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="DF20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="DI20" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="CL21" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="22" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+      <c r="CO21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="CQ21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="CU21" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="DA21" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="DF21" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="DI21" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="CL22" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" spans="1:91" ht="29" x14ac:dyDescent="0.35">
+      <c r="CO22" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="CQ22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CU22" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="DA22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="DF22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DI22" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="CL23" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:91" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+      <c r="CO23" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="CQ23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR23" s="8"/>
+      <c r="CU23" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="DA23" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="DF23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="DI23" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:123" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="CL24" s="4" t="s">
-        <v>156</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="CO24" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="CQ24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="CU24" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="DA24" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="DF24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI24" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CO25" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CQ25" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="CU25" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DA25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="DF25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="DI25" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CO26" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="CQ26" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="CU26" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="DA26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DF26" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="DI26" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CO27" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="CQ27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="CU27" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="DF27" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="DI27" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CO28" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="CQ28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CU28" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="DF28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI28" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:123" ht="45" x14ac:dyDescent="0.25">
+      <c r="CQ29" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU29" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="DF29" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CQ30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CU30" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="DF30" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:123" x14ac:dyDescent="0.25">
+      <c r="CQ31" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="CU31" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:123" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU32" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU33" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU34" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU35" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU36" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU37" s="18" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="99:99" ht="45" x14ac:dyDescent="0.25">
+      <c r="CU38" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU39" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="99:99" ht="45" x14ac:dyDescent="0.25">
+      <c r="CU40" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="99:99" ht="45" x14ac:dyDescent="0.25">
+      <c r="CU41" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU42" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU43" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU44" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU45" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU46" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU47" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="99:99" ht="45" x14ac:dyDescent="0.25">
+      <c r="CU48" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU49" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="99:99" ht="45" x14ac:dyDescent="0.25">
+      <c r="CU50" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU51" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU52" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU53" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU54" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU55" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU56" s="18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="99:99" ht="30" x14ac:dyDescent="0.25">
+      <c r="CU57" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="99:99" x14ac:dyDescent="0.25">
+      <c r="CU58" s="16"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -3195,31 +5017,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2138B4BB-1FBE-4241-B04B-F13088DD4D66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE1A7945-433B-403C-8615-51141F3AC5C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{788B8EDF-F0B2-40C7-AFA4-85C800D88023}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3235,4 +5048,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2138B4BB-1FBE-4241-B04B-F13088DD4D66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE1A7945-433B-403C-8615-51141F3AC5C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed problem with annotations
</commit_message>
<xml_diff>
--- a/grouped table of annotations.xlsx
+++ b/grouped table of annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FC6D12-ED4E-4DDD-8D21-727BF45B2EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83087B2-331E-4FD8-A40E-A7AADDE7E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="5760" windowWidth="28800" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,9 +453,6 @@
     <t>Assign resource to each activity</t>
   </si>
   <si>
-    <t>Represent heatmaps</t>
-  </si>
-  <si>
     <t>Calculate cycle time of only a subset of pairs of events for each subset of traces</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>Identify activity with biggest backlog</t>
   </si>
   <si>
-    <t>Represent scatterplot</t>
-  </si>
-  <si>
     <t>Calculate average of activities per trace</t>
   </si>
   <si>
@@ -507,9 +501,6 @@
     <t>Filter activities by frequency</t>
   </si>
   <si>
-    <t>Represent density of cycle time</t>
-  </si>
-  <si>
     <t>Group traces by year</t>
   </si>
   <si>
@@ -624,9 +615,6 @@
     <t>Calculate frequency of sub-processes</t>
   </si>
   <si>
-    <t>Represent linear tendency of cycle time</t>
-  </si>
-  <si>
     <t>A19 P1 BPI 2017</t>
   </si>
   <si>
@@ -847,6 +835,18 @@
   </si>
   <si>
     <t>Find sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
+  </si>
+  <si>
+    <t>Represent scatterplot of cycle time and an attribute</t>
+  </si>
+  <si>
+    <t>Represent linear tendency of cycle time with respect an attribute</t>
+  </si>
+  <si>
+    <t>Represent heat maps of cycle time and an attribute</t>
+  </si>
+  <si>
+    <t>Represent density diagram of cycle time</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AW4" sqref="AW4"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="BD6" sqref="BD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,492 +1701,492 @@
         <v>89</v>
       </c>
       <c r="CM1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="CN1" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="CN1" s="7" t="s">
-        <v>190</v>
-      </c>
       <c r="CO1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="CP1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="CQ1" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="CP1" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="CQ1" s="7" t="s">
-        <v>201</v>
-      </c>
       <c r="CR1" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="CS1" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="CT1" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="CU1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="CV1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="CW1" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="CX1" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="CY1" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="CV1" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="CW1" s="7" t="s">
+      <c r="CZ1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="CX1" s="7" t="s">
+      <c r="DA1" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="CY1" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="CZ1" s="7" t="s">
+      <c r="DB1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="DC1" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="DA1" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB1" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="DC1" s="11" t="s">
+      <c r="DD1" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="DD1" s="7" t="s">
-        <v>224</v>
-      </c>
       <c r="DE1" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="DF1" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="DG1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="DG1" s="7" t="s">
+      <c r="DH1" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="DI1" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="DJ1" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="DK1" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="DH1" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="DI1" s="7" t="s">
+      <c r="DL1" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="DJ1" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="DK1" s="7" t="s">
+      <c r="DM1" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="DL1" s="7" t="s">
+      <c r="DN1" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="DM1" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="DN1" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="DO1" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="DP1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="DQ1" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="DR1" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="DS1" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="DT1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="DQ1" s="7" t="s">
+      <c r="DU1" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="DR1" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="DS1" s="7" t="s">
+      <c r="DV1" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="DT1" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="DU1" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="DV1" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:126" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="W2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="X2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Y2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Z2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AA2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AB2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AC2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AD2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AE2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AF2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AG2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AH2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AI2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AJ2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AK2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AL2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AM2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AN2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AO2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AP2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AQ2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AR2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AS2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AT2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AU2" s="21" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AV2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AW2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AX2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AY2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AZ2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BA2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="BB2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BC2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="BD2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="BE2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BF2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BG2" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="BH2" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BI2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BJ2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BK2" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BL2" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BM2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BN2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BO2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BP2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BQ2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BR2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BS2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BT2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BU2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BV2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BW2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="BX2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BY2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="BZ2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CA2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CB2" s="22" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="CC2" s="22" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="CD2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CE2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CF2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CG2" s="22" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CH2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CI2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CJ2" s="22" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="CK2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CL2" s="22" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CM2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="CN2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CO2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CP2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="CQ2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CR2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CS2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CT2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CU2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CV2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CW2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CX2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CY2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="CZ2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DA2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DB2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DC2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DD2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DE2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="DF2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DG2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DH2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DI2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DJ2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DK2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DL2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DM2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DN2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DO2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DP2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DQ2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DR2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="DS2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DT2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DU2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="DV2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:126" ht="90" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
         <v>99</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AH3" s="4" t="s">
         <v>91</v>
@@ -2320,7 +2320,7 @@
         <v>91</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AS3" s="4" t="s">
         <v>99</v>
@@ -2473,7 +2473,7 @@
         <v>106</v>
       </c>
       <c r="CQ3" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="CR3" s="4" t="s">
         <v>91</v>
@@ -2482,28 +2482,28 @@
         <v>104</v>
       </c>
       <c r="CT3" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="CU3" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="CV3" s="4" t="s">
         <v>100</v>
       </c>
       <c r="CW3" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="CX3" s="4" t="s">
         <v>90</v>
       </c>
       <c r="CY3" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="CZ3" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="DA3" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DB3" s="4" t="s">
         <v>99</v>
@@ -2518,10 +2518,10 @@
         <v>101</v>
       </c>
       <c r="DF3" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="DG3" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="DH3" s="4" t="s">
         <v>103</v>
@@ -2536,16 +2536,16 @@
         <v>95</v>
       </c>
       <c r="DL3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="DM3" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="DN3" s="4" t="s">
         <v>122</v>
       </c>
       <c r="DO3" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="DP3" s="4" t="s">
         <v>98</v>
@@ -2554,13 +2554,13 @@
         <v>95</v>
       </c>
       <c r="DR3" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="DS3" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="DT3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="DU3" s="4" t="s">
         <v>100</v>
@@ -2569,7 +2569,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:126" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:126" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -2631,16 +2631,16 @@
         <v>127</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Z4" t="s">
         <v>128</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AB4" s="4" t="s">
         <v>126</v>
@@ -2649,19 +2649,19 @@
         <v>100</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="AE4" t="s">
         <v>126</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AG4" t="s">
         <v>114</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AI4" s="4" t="s">
         <v>122</v>
@@ -2670,7 +2670,7 @@
         <v>129</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AL4" s="4" t="s">
         <v>128</v>
@@ -2679,7 +2679,7 @@
         <v>114</v>
       </c>
       <c r="AN4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AO4" s="4" t="s">
         <v>99</v>
@@ -2691,7 +2691,7 @@
         <v>130</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AT4" s="4" t="s">
         <v>103</v>
@@ -2703,7 +2703,7 @@
         <v>132</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="AX4" s="4" t="s">
         <v>127</v>
@@ -2781,7 +2781,7 @@
         <v>115</v>
       </c>
       <c r="BX4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BY4" s="4" t="s">
         <v>116</v>
@@ -2796,10 +2796,10 @@
         <v>138</v>
       </c>
       <c r="CC4" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="CD4" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="CD4" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="CE4" s="4" t="s">
         <v>132</v>
@@ -2829,22 +2829,22 @@
         <v>106</v>
       </c>
       <c r="CN4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CO4" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CP4" s="4" t="s">
         <v>90</v>
       </c>
       <c r="CQ4" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CR4" s="4" t="s">
         <v>122</v>
       </c>
       <c r="CS4" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="CT4" s="4" t="s">
         <v>133</v>
@@ -2856,10 +2856,10 @@
         <v>99</v>
       </c>
       <c r="CW4" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CX4" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CY4" s="4" t="s">
         <v>129</v>
@@ -2874,13 +2874,13 @@
         <v>134</v>
       </c>
       <c r="DC4" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="DD4" s="12" t="s">
         <v>90</v>
       </c>
       <c r="DE4" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="DF4" s="4" t="s">
         <v>133</v>
@@ -2898,10 +2898,10 @@
         <v>108</v>
       </c>
       <c r="DK4" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="DL4" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="DM4" s="4" t="s">
         <v>108</v>
@@ -2913,7 +2913,7 @@
         <v>134</v>
       </c>
       <c r="DQ4" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="DR4" s="4" t="s">
         <v>115</v>
@@ -2925,10 +2925,10 @@
         <v>95</v>
       </c>
       <c r="DU4" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DV4" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:126" ht="75" x14ac:dyDescent="0.25">
@@ -2939,7 +2939,7 @@
         <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H5" t="s">
         <v>90</v>
@@ -2954,16 +2954,16 @@
         <v>132</v>
       </c>
       <c r="N5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q5" t="s">
         <v>107</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>129</v>
@@ -2972,31 +2972,31 @@
         <v>99</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AA5" t="s">
         <v>114</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AG5" s="4" t="s">
         <v>127</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AK5" s="4" t="s">
         <v>99</v>
       </c>
       <c r="AL5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AM5" s="4" t="s">
         <v>132</v>
@@ -3005,13 +3005,13 @@
         <v>137</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AT5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AU5" s="4" t="s">
         <v>106</v>
@@ -3020,7 +3020,7 @@
         <v>99</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AX5" s="4" t="s">
         <v>106</v>
@@ -3029,7 +3029,7 @@
         <v>119</v>
       </c>
       <c r="AZ5" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="BA5" s="4" t="s">
         <v>92</v>
@@ -3065,7 +3065,7 @@
         <v>121</v>
       </c>
       <c r="BM5" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BN5" s="4" t="s">
         <v>104</v>
@@ -3077,13 +3077,13 @@
         <v>116</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BR5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BS5" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="BS5" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="BT5" s="4" t="s">
         <v>133</v>
@@ -3098,7 +3098,7 @@
         <v>134</v>
       </c>
       <c r="BX5" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BY5" s="4" t="s">
         <v>115</v>
@@ -3110,7 +3110,7 @@
         <v>90</v>
       </c>
       <c r="CB5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="CC5" s="4" t="s">
         <v>101</v>
@@ -3119,7 +3119,7 @@
         <v>126</v>
       </c>
       <c r="CE5" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CF5" s="4" t="s">
         <v>104</v>
@@ -3137,7 +3137,7 @@
         <v>135</v>
       </c>
       <c r="CK5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="CL5" s="4" t="s">
         <v>114</v>
@@ -3152,22 +3152,22 @@
         <v>94</v>
       </c>
       <c r="CP5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CQ5" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="CS5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="CT5" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="CU5" s="4" t="s">
         <v>122</v>
       </c>
       <c r="CV5" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CW5" s="4" t="s">
         <v>95</v>
@@ -3179,25 +3179,25 @@
         <v>121</v>
       </c>
       <c r="DA5" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DB5" s="4" t="s">
         <v>96</v>
       </c>
       <c r="DC5" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="DD5" s="13" t="s">
         <v>95</v>
       </c>
       <c r="DE5" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="DF5" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DG5" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="DH5" s="4" t="s">
         <v>129</v>
@@ -3209,39 +3209,39 @@
         <v>121</v>
       </c>
       <c r="DK5" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="DM5" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DO5" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DP5" s="3" t="s">
         <v>135</v>
       </c>
       <c r="DR5" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DS5" s="4" t="s">
         <v>95</v>
       </c>
       <c r="DT5" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="DU5" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DV5" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:126" ht="90" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>151</v>
+    <row r="6" spans="1:126" ht="75" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="K6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N6" t="s">
         <v>114</v>
@@ -3250,28 +3250,28 @@
         <v>137</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="V6" t="s">
         <v>121</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AM6" s="4" t="s">
         <v>104</v>
       </c>
       <c r="AO6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AV6" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="AT6" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="AU6" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="AV6" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="AW6" s="4" t="s">
         <v>122</v>
@@ -3283,7 +3283,7 @@
         <v>108</v>
       </c>
       <c r="AZ6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="BA6" s="4" t="s">
         <v>109</v>
@@ -3292,10 +3292,10 @@
         <v>92</v>
       </c>
       <c r="BD6" s="4" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="BF6" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="BG6" s="4" t="s">
         <v>93</v>
@@ -3319,10 +3319,10 @@
         <v>116</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BQ6" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BR6" s="4" t="s">
         <v>116</v>
@@ -3337,7 +3337,7 @@
         <v>114</v>
       </c>
       <c r="BV6" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="BW6" s="4" t="s">
         <v>90</v>
@@ -3352,10 +3352,10 @@
         <v>127</v>
       </c>
       <c r="CA6" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CB6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="CC6" s="4" t="s">
         <v>125</v>
@@ -3364,7 +3364,7 @@
         <v>122</v>
       </c>
       <c r="CE6" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="CF6" s="4" t="s">
         <v>105</v>
@@ -3376,16 +3376,16 @@
         <v>134</v>
       </c>
       <c r="CI6" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CJ6" s="4" t="s">
         <v>104</v>
       </c>
       <c r="CK6" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="CL6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CM6" s="8" t="s">
         <v>122</v>
@@ -3421,19 +3421,19 @@
         <v>114</v>
       </c>
       <c r="DB6" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DC6" s="14" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="DD6" s="12" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="DE6" s="15" t="s">
         <v>134</v>
       </c>
       <c r="DF6" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="DG6" s="15" t="s">
         <v>122</v>
@@ -3451,27 +3451,27 @@
         <v>95</v>
       </c>
       <c r="DM6" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="DO6" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="DO6" s="15" t="s">
-        <v>244</v>
-      </c>
       <c r="DR6" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="DS6" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DV6" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:126" ht="90" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:126" ht="75" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
         <v>134</v>
       </c>
-      <c r="N7" t="s">
-        <v>151</v>
+      <c r="N7" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="U7" t="s">
         <v>103</v>
@@ -3486,7 +3486,7 @@
         <v>114</v>
       </c>
       <c r="AO7" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AT7" s="4" t="s">
         <v>129</v>
@@ -3495,19 +3495,19 @@
         <v>111</v>
       </c>
       <c r="AX7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AY7" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AZ7" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="BA7" s="4" t="s">
         <v>127</v>
       </c>
       <c r="BC7" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="BF7" s="4" t="s">
         <v>104</v>
@@ -3519,28 +3519,28 @@
         <v>122</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BM7" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BO7" s="4" t="s">
         <v>99</v>
       </c>
       <c r="BP7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BQ7" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="BR7" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BS7" s="4" t="s">
         <v>98</v>
       </c>
       <c r="BT7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BU7" s="4" t="s">
         <v>108</v>
@@ -3561,67 +3561,67 @@
         <v>99</v>
       </c>
       <c r="CB7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CC7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CD7" s="4" t="s">
         <v>104</v>
       </c>
       <c r="CE7" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CF7" s="4" t="s">
         <v>109</v>
       </c>
       <c r="CG7" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="CH7" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CI7" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="CJ7" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CK7" s="4" t="s">
         <v>127</v>
       </c>
       <c r="CL7" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="CM7" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="CN7" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="CO7" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="CP7" s="8" t="s">
         <v>119</v>
       </c>
       <c r="CQ7" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CS7" s="8" t="s">
         <v>92</v>
       </c>
       <c r="CT7" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="CV7" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="CW7" s="18" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="CX7" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CZ7" s="8" t="s">
         <v>90</v>
@@ -3630,16 +3630,16 @@
         <v>104</v>
       </c>
       <c r="DC7" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="DD7" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="DE7" s="8" t="s">
         <v>104</v>
       </c>
       <c r="DF7" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="DG7" s="8" t="s">
         <v>106</v>
@@ -3648,19 +3648,19 @@
         <v>134</v>
       </c>
       <c r="DI7" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="DM7" s="8" t="s">
         <v>108</v>
       </c>
       <c r="DO7" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="DR7" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="DS7" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DV7" s="4" t="s">
         <v>112</v>
@@ -3668,13 +3668,13 @@
     </row>
     <row r="8" spans="1:126" ht="90" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U8" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="V8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AI8" s="4" t="s">
         <v>114</v>
@@ -3683,25 +3683,25 @@
         <v>132</v>
       </c>
       <c r="AO8" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AT8" s="4" t="s">
         <v>122</v>
       </c>
       <c r="AV8" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AX8" s="4" t="s">
         <v>99</v>
       </c>
       <c r="AY8" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AZ8" s="4" t="s">
         <v>121</v>
       </c>
       <c r="BC8" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="BF8" s="4" t="s">
         <v>108</v>
@@ -3710,7 +3710,7 @@
         <v>106</v>
       </c>
       <c r="BK8" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="BM8" s="4" t="s">
         <v>112</v>
@@ -3719,10 +3719,10 @@
         <v>112</v>
       </c>
       <c r="BP8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ8" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="BQ8" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="BR8" s="4" t="s">
         <v>116</v>
@@ -3731,7 +3731,7 @@
         <v>116</v>
       </c>
       <c r="BT8" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BU8" s="4" t="s">
         <v>99</v>
@@ -3740,19 +3740,19 @@
         <v>121</v>
       </c>
       <c r="BW8" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="BY8" s="4" t="s">
         <v>115</v>
       </c>
       <c r="BZ8" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CD8" s="4" t="s">
         <v>121</v>
       </c>
       <c r="CE8" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="CF8" s="4" t="s">
         <v>115</v>
@@ -3761,22 +3761,22 @@
         <v>129</v>
       </c>
       <c r="CI8" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="CJ8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CK8" s="4" t="s">
         <v>125</v>
       </c>
       <c r="CL8" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="CM8" s="8" t="s">
         <v>119</v>
       </c>
       <c r="CN8" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CO8" s="8" t="s">
         <v>116</v>
@@ -3791,16 +3791,16 @@
         <v>92</v>
       </c>
       <c r="CT8" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CV8" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="CW8" s="4" t="s">
         <v>95</v>
       </c>
       <c r="CX8" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="CZ8" s="8" t="s">
         <v>106</v>
@@ -3812,37 +3812,37 @@
         <v>108</v>
       </c>
       <c r="DD8" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="DE8" s="8" t="s">
         <v>134</v>
       </c>
       <c r="DF8" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DG8" s="8" t="s">
         <v>119</v>
       </c>
       <c r="DH8" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="DI8" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="DM8" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DO8" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DR8" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DS8" s="8" t="s">
         <v>111</v>
       </c>
       <c r="DV8" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:126" ht="75" x14ac:dyDescent="0.25">
@@ -3853,7 +3853,7 @@
         <v>127</v>
       </c>
       <c r="V9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AV9" s="4" t="s">
         <v>99</v>
@@ -3886,13 +3886,13 @@
         <v>116</v>
       </c>
       <c r="BR9" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BS9" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BU9" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BV9" s="4" t="s">
         <v>101</v>
@@ -3904,7 +3904,7 @@
         <v>121</v>
       </c>
       <c r="BZ9" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="CD9" s="4" t="s">
         <v>124</v>
@@ -3913,7 +3913,7 @@
         <v>106</v>
       </c>
       <c r="CF9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CG9" s="4" t="s">
         <v>134</v>
@@ -3943,46 +3943,46 @@
         <v>99</v>
       </c>
       <c r="CQ9" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CS9" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="CT9" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="CV9" s="8" t="s">
         <v>134</v>
       </c>
       <c r="CW9" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="CX9" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CZ9" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="DB9" s="8" t="s">
         <v>104</v>
       </c>
       <c r="DC9" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="DD9" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="DE9" s="8" t="s">
         <v>115</v>
       </c>
       <c r="DG9" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="DH9" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="DM9" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DO9" s="8" t="s">
         <v>115</v>
@@ -3994,33 +3994,33 @@
         <v>106</v>
       </c>
       <c r="DV9" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:126" ht="90" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="U10" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="V10" t="s">
         <v>106</v>
       </c>
       <c r="AY10" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AZ10" s="4" t="s">
         <v>122</v>
       </c>
       <c r="BC10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="BF10" s="4" t="s">
         <v>134</v>
       </c>
       <c r="BM10" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BO10" s="4" t="s">
         <v>110</v>
@@ -4029,7 +4029,7 @@
         <v>94</v>
       </c>
       <c r="BQ10" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="BS10" s="4" t="s">
         <v>136</v>
@@ -4047,19 +4047,19 @@
         <v>110</v>
       </c>
       <c r="CD10" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="CF10" s="4" t="s">
         <v>109</v>
       </c>
       <c r="CG10" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CI10" s="4" t="s">
         <v>108</v>
       </c>
       <c r="CK10" s="4" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="CL10" s="4" t="s">
         <v>134</v>
@@ -4071,7 +4071,7 @@
         <v>134</v>
       </c>
       <c r="CO10" s="20" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="CP10" s="8" t="s">
         <v>121</v>
@@ -4080,25 +4080,25 @@
         <v>92</v>
       </c>
       <c r="CS10" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CT10" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="CV10" s="8" t="s">
         <v>102</v>
       </c>
       <c r="CX10" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="CZ10" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="DB10" s="8" t="s">
         <v>134</v>
       </c>
       <c r="DC10" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="DD10" s="4" t="s">
         <v>119</v>
@@ -4113,13 +4113,13 @@
         <v>121</v>
       </c>
       <c r="DM10" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DO10" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DR10" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DS10" s="12" t="s">
         <v>104</v>
@@ -4139,7 +4139,7 @@
         <v>121</v>
       </c>
       <c r="AZ11" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="BM11" s="4" t="s">
         <v>106</v>
@@ -4151,13 +4151,13 @@
         <v>116</v>
       </c>
       <c r="BQ11" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="BS11" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BU11" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="BW11" s="4" t="s">
         <v>132</v>
@@ -4166,28 +4166,28 @@
         <v>116</v>
       </c>
       <c r="CD11" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="CF11" s="4" t="s">
         <v>125</v>
       </c>
       <c r="CG11" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CI11" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="CK11" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="CL11" s="4" t="s">
         <v>104</v>
       </c>
       <c r="CM11" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="CN11" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="CO11" s="8" t="s">
         <v>122</v>
@@ -4199,7 +4199,7 @@
         <v>104</v>
       </c>
       <c r="CT11" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CV11" s="8" t="s">
         <v>99</v>
@@ -4214,7 +4214,7 @@
         <v>129</v>
       </c>
       <c r="DC11" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="DD11" s="4" t="s">
         <v>108</v>
@@ -4223,7 +4223,7 @@
         <v>104</v>
       </c>
       <c r="DG11" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="DH11" s="8" t="s">
         <v>134</v>
@@ -4232,16 +4232,16 @@
         <v>135</v>
       </c>
       <c r="DO11" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="DR11" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="DS11" s="8" t="s">
         <v>134</v>
       </c>
       <c r="DV11" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:126" ht="90" x14ac:dyDescent="0.25">
@@ -4249,13 +4249,13 @@
         <v>106</v>
       </c>
       <c r="U12" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="AY12" s="4" t="s">
         <v>122</v>
       </c>
       <c r="BM12" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="BO12" s="4" t="s">
         <v>99</v>
@@ -4270,16 +4270,16 @@
         <v>106</v>
       </c>
       <c r="BZ12" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="CF12" s="4" t="s">
         <v>109</v>
       </c>
       <c r="CG12" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="CI12" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CK12" s="4" t="s">
         <v>109</v>
@@ -4288,10 +4288,10 @@
         <v>134</v>
       </c>
       <c r="CM12" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="CN12" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="CO12" s="8" t="s">
         <v>106</v>
@@ -4303,25 +4303,25 @@
         <v>92</v>
       </c>
       <c r="CT12" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="CV12" s="8" t="s">
         <v>129</v>
       </c>
       <c r="CX12" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CZ12" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="DB12" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="DC12" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="DD12" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="DE12" s="8" t="s">
         <v>134</v>
@@ -4353,7 +4353,7 @@
         <v>104</v>
       </c>
       <c r="AY13" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="BM13" s="4" t="s">
         <v>134</v>
@@ -4368,10 +4368,10 @@
         <v>126</v>
       </c>
       <c r="CG13" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CI13" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CK13" s="4" t="s">
         <v>121</v>
@@ -4383,19 +4383,19 @@
         <v>95</v>
       </c>
       <c r="CN13" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="CO13" s="8" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="CP13" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CQ13" s="8" t="s">
         <v>127</v>
       </c>
       <c r="CT13" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="CX13" s="19" t="s">
         <v>134</v>
@@ -4405,10 +4405,10 @@
       </c>
       <c r="DB13" s="10"/>
       <c r="DC13" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="DD13" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DE13" s="8" t="s">
         <v>104</v>
@@ -4420,19 +4420,19 @@
         <v>108</v>
       </c>
       <c r="DM13" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DO13" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DR13" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DS13" s="8" t="s">
         <v>134</v>
       </c>
       <c r="DV13" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:126" ht="75" x14ac:dyDescent="0.25">
@@ -4440,22 +4440,22 @@
         <v>122</v>
       </c>
       <c r="AY14" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="BM14" s="4" t="s">
         <v>129</v>
       </c>
       <c r="BP14" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CG14" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CI14" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CK14" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="CL14" s="4" t="s">
         <v>120</v>
@@ -4470,31 +4470,31 @@
         <v>106</v>
       </c>
       <c r="CP14" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="CQ14" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="CT14" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="CT14" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="CX14" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CZ14" s="4" t="s">
         <v>135</v>
       </c>
       <c r="DC14" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="DD14" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="DE14" s="8" t="s">
         <v>134</v>
       </c>
       <c r="DG14" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="DH14" s="8" t="s">
         <v>119</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="15" spans="1:126" ht="60" x14ac:dyDescent="0.25">
       <c r="AY15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BP15" s="4" t="s">
         <v>121</v>
@@ -4520,16 +4520,16 @@
         <v>101</v>
       </c>
       <c r="CK15" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="CL15" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="CN15" s="8" t="s">
         <v>121</v>
       </c>
       <c r="CO15" s="8" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="CP15" s="8" t="s">
         <v>121</v>
@@ -4538,7 +4538,7 @@
         <v>121</v>
       </c>
       <c r="CT15" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="CX15" s="19" t="s">
         <v>134</v>
@@ -4547,30 +4547,30 @@
         <v>121</v>
       </c>
       <c r="DC15" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="DD15" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="DE15" s="8" t="s">
         <v>104</v>
       </c>
       <c r="DG15" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="DH15" s="4" t="s">
         <v>108</v>
       </c>
       <c r="DO15" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DR15" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:126" ht="75" x14ac:dyDescent="0.25">
       <c r="AY16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BP16" s="4" t="s">
         <v>134</v>
@@ -4582,22 +4582,22 @@
         <v>99</v>
       </c>
       <c r="CK16" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="CL16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CN16" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="CP16" s="8" t="s">
         <v>101</v>
       </c>
       <c r="CQ16" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CT16" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="CX16" s="18" t="s">
         <v>99</v>
@@ -4615,33 +4615,33 @@
         <v>126</v>
       </c>
       <c r="DO16" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="DR16" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="51:122" ht="75" x14ac:dyDescent="0.25">
       <c r="AY17" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="BP17" s="4" t="s">
         <v>104</v>
       </c>
       <c r="CG17" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="CI17" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="CK17" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="CL17" s="4" t="s">
         <v>121</v>
       </c>
       <c r="CN17" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CP17" s="8" t="s">
         <v>99</v>
@@ -4650,7 +4650,7 @@
         <v>121</v>
       </c>
       <c r="CT17" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CX17" s="9"/>
       <c r="CZ17" s="8" t="s">
@@ -4666,27 +4666,27 @@
         <v>95</v>
       </c>
       <c r="DO17" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="DR17" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="51:122" ht="45" x14ac:dyDescent="0.25">
       <c r="AY18" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="CG18" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CI18" s="4" t="s">
         <v>115</v>
       </c>
       <c r="CK18" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="CL18" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="CN18" s="8" t="s">
         <v>121</v>
@@ -4695,14 +4695,14 @@
         <v>121</v>
       </c>
       <c r="CQ18" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CT18" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="CX18" s="9"/>
       <c r="CZ18" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="DE18" s="8" t="s">
         <v>134</v>
@@ -4711,18 +4711,18 @@
         <v>129</v>
       </c>
       <c r="DO18" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="DR18" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="51:122" ht="30" x14ac:dyDescent="0.25">
       <c r="CG19" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="CI19" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="CK19" s="4" t="s">
         <v>109</v>
@@ -4740,7 +4740,7 @@
         <v>92</v>
       </c>
       <c r="CT19" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="CZ19" s="8" t="s">
         <v>134</v>
@@ -4752,21 +4752,21 @@
         <v>119</v>
       </c>
       <c r="DO19" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="DR19" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="51:122" ht="45" x14ac:dyDescent="0.25">
       <c r="CG20" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CK20" s="4" t="s">
         <v>119</v>
       </c>
       <c r="CN20" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="CP20" s="8" t="s">
         <v>129</v>
@@ -4775,7 +4775,7 @@
         <v>104</v>
       </c>
       <c r="CT20" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CZ20" s="8" t="s">
         <v>110</v>
@@ -4787,36 +4787,36 @@
         <v>137</v>
       </c>
       <c r="DO20" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="DR20" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="51:122" ht="60" x14ac:dyDescent="0.25">
       <c r="CG21" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CK21" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CN21" s="8" t="s">
         <v>99</v>
       </c>
       <c r="CP21" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="CQ21" s="18" t="s">
         <v>92</v>
       </c>
       <c r="CT21" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="CZ21" s="8" t="s">
         <v>129</v>
       </c>
       <c r="DE21" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="DH21" s="4" t="s">
         <v>119</v>
@@ -4833,7 +4833,7 @@
         <v>101</v>
       </c>
       <c r="CT22" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CZ22" s="8" t="s">
         <v>129</v>
@@ -4850,13 +4850,13 @@
         <v>121</v>
       </c>
       <c r="CN23" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="CP23" s="8" t="s">
         <v>99</v>
       </c>
       <c r="CT23" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="CZ23" s="8" t="s">
         <v>127</v>
@@ -4865,25 +4865,25 @@
         <v>115</v>
       </c>
       <c r="DH23" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="51:122" ht="45" x14ac:dyDescent="0.25">
       <c r="CK24" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="CN24" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CP24" s="8" t="s">
         <v>106</v>
       </c>
       <c r="CQ24" s="8"/>
       <c r="CT24" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="CZ24" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="DE24" s="8" t="s">
         <v>108</v>
@@ -4892,18 +4892,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="51:122" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="51:122" ht="60" x14ac:dyDescent="0.25">
       <c r="CK25" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="CN25" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="CN25" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="CP25" s="8" t="s">
         <v>129</v>
       </c>
       <c r="CT25" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="CZ25" s="8" t="s">
         <v>134</v>
@@ -4920,10 +4920,10 @@
         <v>134</v>
       </c>
       <c r="CP26" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="CT26" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="CZ26" s="8" t="s">
         <v>110</v>
@@ -4937,13 +4937,13 @@
     </row>
     <row r="27" spans="51:122" ht="30" x14ac:dyDescent="0.25">
       <c r="CN27" s="8" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="CP27" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CT27" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CZ27" s="2" t="s">
         <v>106</v>
@@ -4957,30 +4957,30 @@
     </row>
     <row r="28" spans="51:122" ht="30" x14ac:dyDescent="0.25">
       <c r="CN28" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="CP28" s="8" t="s">
         <v>101</v>
       </c>
       <c r="CT28" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="DE28" s="8" t="s">
         <v>111</v>
       </c>
       <c r="DH28" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="51:122" ht="30" x14ac:dyDescent="0.25">
       <c r="CN29" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="CP29" s="8" t="s">
         <v>99</v>
       </c>
       <c r="CT29" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="DE29" s="8" t="s">
         <v>109</v>
@@ -4994,7 +4994,7 @@
         <v>127</v>
       </c>
       <c r="CT30" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="DE30" s="8" t="s">
         <v>121</v>
@@ -5005,28 +5005,28 @@
         <v>99</v>
       </c>
       <c r="CT31" s="17" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="DE31" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="51:122" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="51:122" ht="30" x14ac:dyDescent="0.25">
       <c r="CP32" s="8" t="s">
         <v>116</v>
       </c>
       <c r="CT32" s="8" t="s">
-        <v>151</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT33" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="98:98" x14ac:dyDescent="0.25">
       <c r="CT34" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="98:98" x14ac:dyDescent="0.25">
@@ -5041,12 +5041,12 @@
     </row>
     <row r="37" spans="98:98" x14ac:dyDescent="0.25">
       <c r="CT37" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="98:98" x14ac:dyDescent="0.25">
       <c r="CT38" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="98:98" ht="45" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
     </row>
     <row r="40" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT40" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="98:98" ht="45" x14ac:dyDescent="0.25">
@@ -5066,37 +5066,37 @@
     </row>
     <row r="42" spans="98:98" ht="45" x14ac:dyDescent="0.25">
       <c r="CT42" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT43" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT44" s="18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT45" s="18" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT46" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT47" s="18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT48" s="18" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="98:98" ht="45" x14ac:dyDescent="0.25">
@@ -5106,32 +5106,32 @@
     </row>
     <row r="50" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT50" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="98:98" ht="45" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="98:98" ht="60" x14ac:dyDescent="0.25">
       <c r="CT51" s="18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT52" s="18" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT53" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT54" s="17" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="55" spans="98:98" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT55" s="18" t="s">
-        <v>151</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="98:98" x14ac:dyDescent="0.25">
@@ -5141,12 +5141,12 @@
     </row>
     <row r="57" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT57" s="18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="98:98" ht="30" x14ac:dyDescent="0.25">
       <c r="CT58" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="98:98" x14ac:dyDescent="0.25">
@@ -5160,12 +5160,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -5349,6 +5343,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5359,22 +5359,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2138B4BB-1FBE-4241-B04B-F13088DD4D66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{788B8EDF-F0B2-40C7-AFA4-85C800D88023}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5392,6 +5376,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2138B4BB-1FBE-4241-B04B-F13088DD4D66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE1A7945-433B-403C-8615-51141F3AC5C5}">
   <ds:schemaRefs>

</xml_diff>